<commit_message>
Obisidian vault manual backup: 26-03-2025 16:59:45 on macbook-air-de-felix. 2 files edited
</commit_message>
<xml_diff>
--- a/ISEN/Microéconomie/CIPA3/FISA3 - Microéconomie - Exercice Annuités - Mar25 vETUDIANT.xlsx
+++ b/ISEN/Microéconomie/CIPA3/FISA3 - Microéconomie - Exercice Annuités - Mar25 vETUDIANT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixmarquet/Nextcloud/Documents/ISEN/Cours/Obsidian Vault/ISEN/Microéconomie/CIPA3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB747C7F-01DB-DA4D-8A6C-0020C7F2280B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD6AFDD-0087-5B45-8F23-5CCBF53C9129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="22460" xr2:uid="{A8BAD0AD-D584-4C72-A389-BC1D156E0E55}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>CCR</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>https://www.meilleurtaux.com/credit-immobilier/notre-analyse-des-taux.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -967,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A74228A-9D4A-4EAA-9887-D3B2960D0618}">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScale="144" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2437,7 +2440,7 @@
         <v>2</v>
       </c>
       <c r="B56" s="5">
-        <f>B55-E55</f>
+        <f>B55+D55</f>
         <v>20600</v>
       </c>
       <c r="C56" s="5">
@@ -2476,7 +2479,7 @@
         <v>3</v>
       </c>
       <c r="B57" s="5">
-        <f t="shared" ref="B57:B59" si="17">B56-E56</f>
+        <f t="shared" ref="B57:B59" si="17">B56+D56</f>
         <v>21218</v>
       </c>
       <c r="C57" s="5">
@@ -2567,6 +2570,11 @@
       <c r="L59" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>